<commit_message>
0806update with new notebook version
</commit_message>
<xml_diff>
--- a/PycharmCodes_xlsxFiles/data_return_0726.xlsx
+++ b/PycharmCodes_xlsxFiles/data_return_0726.xlsx
@@ -2387,8 +2387,8 @@
   <x:sheetPr codeName="Sheet13"/>
   <x:dimension ref="A1:V8"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="T4" activeCellId="0" sqref="T4:T4"/>
+    <x:sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="S7" activeCellId="0" sqref="S7:S7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.399999999999999"/>
@@ -5838,7 +5838,7 @@
   <x:dimension ref="A1:V8"/>
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="B1" activeCellId="0" sqref="B1:V1"/>
+      <x:selection activeCell="B2" activeCellId="0" sqref="B2:B2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.399999999999999"/>

</xml_diff>